<commit_message>
add contacts report use case
</commit_message>
<xml_diff>
--- a/documents/contacts.xlsx
+++ b/documents/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian\Documents\GitHub\PhoneForge\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83B4D48-3E6F-4184-AB0F-F89422AC0FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD799404-0DC1-4075-A18B-25DF5DFBF379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>jdoe@gmail.com</t>
   </si>
@@ -241,6 +241,210 @@
   </si>
   <si>
     <t>0971234456</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>ecarter@yahoo.com</t>
+  </si>
+  <si>
+    <t>0957642231</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Hartman</t>
+  </si>
+  <si>
+    <t>ohartman@live.com</t>
+  </si>
+  <si>
+    <t>0981616544</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>Mercer</t>
+  </si>
+  <si>
+    <t>jmercer@live.com</t>
+  </si>
+  <si>
+    <t>0998172743</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Davenport</t>
+  </si>
+  <si>
+    <t>cdavenport@gmail.com</t>
+  </si>
+  <si>
+    <t>0917583245</t>
+  </si>
+  <si>
+    <t>Gavin</t>
+  </si>
+  <si>
+    <t>Halstead</t>
+  </si>
+  <si>
+    <t>ghalstead@yahoo.com</t>
+  </si>
+  <si>
+    <t>0927653262</t>
+  </si>
+  <si>
+    <t>Lila</t>
+  </si>
+  <si>
+    <t>Kensington</t>
+  </si>
+  <si>
+    <t>lkensington@gmail.com</t>
+  </si>
+  <si>
+    <t>0921345354</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rowley</t>
+  </si>
+  <si>
+    <t>drowley@live.com</t>
+  </si>
+  <si>
+    <t>0988787977</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Linton</t>
+  </si>
+  <si>
+    <t>hlinton@gmail.com</t>
+  </si>
+  <si>
+    <t>0972134890</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Callahan</t>
+  </si>
+  <si>
+    <t>xcallahan@gmail.com</t>
+  </si>
+  <si>
+    <t>0918765321</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Merritt</t>
+  </si>
+  <si>
+    <t>0996876644</t>
+  </si>
+  <si>
+    <t>Tristan</t>
+  </si>
+  <si>
+    <t>Holloway</t>
+  </si>
+  <si>
+    <t>zmerritt@yahoo.com</t>
+  </si>
+  <si>
+    <t>tholloway@live.com</t>
+  </si>
+  <si>
+    <t>0957987981</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Pennington</t>
+  </si>
+  <si>
+    <t>mpennington@yahoo.com</t>
+  </si>
+  <si>
+    <t>0918374653</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Becket</t>
+  </si>
+  <si>
+    <t>nbecket@live.com</t>
+  </si>
+  <si>
+    <t>0986567214</t>
+  </si>
+  <si>
+    <t>Spencer</t>
+  </si>
+  <si>
+    <t>Aldridge</t>
+  </si>
+  <si>
+    <t>saldridge@gmail.com</t>
+  </si>
+  <si>
+    <t>0916783243</t>
+  </si>
+  <si>
+    <t>Hazel</t>
+  </si>
+  <si>
+    <t>Kingsley</t>
+  </si>
+  <si>
+    <t>hkingsley@gmail.com</t>
+  </si>
+  <si>
+    <t>0992345612</t>
+  </si>
+  <si>
+    <t>Owen</t>
+  </si>
+  <si>
+    <t>Thorne</t>
+  </si>
+  <si>
+    <t>othorne@yahoo.com</t>
+  </si>
+  <si>
+    <t>0916366327</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Prescott</t>
+  </si>
+  <si>
+    <t>aprescott@gmail.com</t>
+  </si>
+  <si>
+    <t>0928764378</t>
   </si>
 </sst>
 </file>
@@ -570,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,6 +1037,244 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -855,8 +1297,25 @@
     <hyperlink ref="C16" r:id="rId16" xr:uid="{CB708ABE-2E24-4234-B0A4-2651A479F21D}"/>
     <hyperlink ref="C17" r:id="rId17" xr:uid="{33AFE8E3-FC8B-4EF1-817F-89905B6343FF}"/>
     <hyperlink ref="C18" r:id="rId18" xr:uid="{59D0B267-36EA-4572-962E-7F9A49D75671}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{431FA698-9548-4AFD-BA35-BFFA574D1EC8}"/>
+    <hyperlink ref="C20" r:id="rId20" xr:uid="{92543B91-8539-4C80-8C6C-A81EF290F680}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{86F255D0-F760-459C-8452-1D1B1EB8CDC5}"/>
+    <hyperlink ref="C22" r:id="rId22" xr:uid="{B150314C-AA6C-46ED-854B-4DDF9E1E86BF}"/>
+    <hyperlink ref="C23" r:id="rId23" xr:uid="{93B541C5-3C41-49A6-A072-314B25F40A55}"/>
+    <hyperlink ref="C24" r:id="rId24" xr:uid="{C374C8A2-580B-42E0-B653-B8F0FF5550ED}"/>
+    <hyperlink ref="C25" r:id="rId25" xr:uid="{833F78B3-8231-466D-8BC6-C4C251235B65}"/>
+    <hyperlink ref="C26" r:id="rId26" xr:uid="{A1CCFB5A-71C9-4C75-A11B-59CF073C5453}"/>
+    <hyperlink ref="C27" r:id="rId27" xr:uid="{E1C6005C-A766-46A7-85C7-95D531E49505}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{FAFD8500-999F-4D3B-A58A-F2F1577A50AE}"/>
+    <hyperlink ref="C28" r:id="rId29" xr:uid="{7EBE2A80-7092-41E7-B4FF-61FDCB68A5FF}"/>
+    <hyperlink ref="C30" r:id="rId30" xr:uid="{F79E5F1F-33E1-4D62-8E17-F1FDD63F43C3}"/>
+    <hyperlink ref="C31" r:id="rId31" xr:uid="{CEE71183-8DFC-47ED-88FA-A00186F99F15}"/>
+    <hyperlink ref="C32" r:id="rId32" xr:uid="{4B004895-5E61-48B7-8E8D-224A77DD19CA}"/>
+    <hyperlink ref="C33" r:id="rId33" xr:uid="{F98998D1-2A3D-4BF9-BD5C-661A0A881EBF}"/>
+    <hyperlink ref="C34" r:id="rId34" xr:uid="{F0D4BB08-1D95-42A5-B2B0-1C3875CE003F}"/>
+    <hyperlink ref="C35" r:id="rId35" xr:uid="{4F374651-5330-4C60-AC93-B51468E32088}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: pdf report generation (#66)
* add contacts report use case

* make contacts report handler sealed
</commit_message>
<xml_diff>
--- a/documents/contacts.xlsx
+++ b/documents/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian\Documents\GitHub\PhoneForge\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83B4D48-3E6F-4184-AB0F-F89422AC0FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD799404-0DC1-4075-A18B-25DF5DFBF379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>jdoe@gmail.com</t>
   </si>
@@ -241,6 +241,210 @@
   </si>
   <si>
     <t>0971234456</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>ecarter@yahoo.com</t>
+  </si>
+  <si>
+    <t>0957642231</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Hartman</t>
+  </si>
+  <si>
+    <t>ohartman@live.com</t>
+  </si>
+  <si>
+    <t>0981616544</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>Mercer</t>
+  </si>
+  <si>
+    <t>jmercer@live.com</t>
+  </si>
+  <si>
+    <t>0998172743</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Davenport</t>
+  </si>
+  <si>
+    <t>cdavenport@gmail.com</t>
+  </si>
+  <si>
+    <t>0917583245</t>
+  </si>
+  <si>
+    <t>Gavin</t>
+  </si>
+  <si>
+    <t>Halstead</t>
+  </si>
+  <si>
+    <t>ghalstead@yahoo.com</t>
+  </si>
+  <si>
+    <t>0927653262</t>
+  </si>
+  <si>
+    <t>Lila</t>
+  </si>
+  <si>
+    <t>Kensington</t>
+  </si>
+  <si>
+    <t>lkensington@gmail.com</t>
+  </si>
+  <si>
+    <t>0921345354</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rowley</t>
+  </si>
+  <si>
+    <t>drowley@live.com</t>
+  </si>
+  <si>
+    <t>0988787977</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Linton</t>
+  </si>
+  <si>
+    <t>hlinton@gmail.com</t>
+  </si>
+  <si>
+    <t>0972134890</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Callahan</t>
+  </si>
+  <si>
+    <t>xcallahan@gmail.com</t>
+  </si>
+  <si>
+    <t>0918765321</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Merritt</t>
+  </si>
+  <si>
+    <t>0996876644</t>
+  </si>
+  <si>
+    <t>Tristan</t>
+  </si>
+  <si>
+    <t>Holloway</t>
+  </si>
+  <si>
+    <t>zmerritt@yahoo.com</t>
+  </si>
+  <si>
+    <t>tholloway@live.com</t>
+  </si>
+  <si>
+    <t>0957987981</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Pennington</t>
+  </si>
+  <si>
+    <t>mpennington@yahoo.com</t>
+  </si>
+  <si>
+    <t>0918374653</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Becket</t>
+  </si>
+  <si>
+    <t>nbecket@live.com</t>
+  </si>
+  <si>
+    <t>0986567214</t>
+  </si>
+  <si>
+    <t>Spencer</t>
+  </si>
+  <si>
+    <t>Aldridge</t>
+  </si>
+  <si>
+    <t>saldridge@gmail.com</t>
+  </si>
+  <si>
+    <t>0916783243</t>
+  </si>
+  <si>
+    <t>Hazel</t>
+  </si>
+  <si>
+    <t>Kingsley</t>
+  </si>
+  <si>
+    <t>hkingsley@gmail.com</t>
+  </si>
+  <si>
+    <t>0992345612</t>
+  </si>
+  <si>
+    <t>Owen</t>
+  </si>
+  <si>
+    <t>Thorne</t>
+  </si>
+  <si>
+    <t>othorne@yahoo.com</t>
+  </si>
+  <si>
+    <t>0916366327</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Prescott</t>
+  </si>
+  <si>
+    <t>aprescott@gmail.com</t>
+  </si>
+  <si>
+    <t>0928764378</t>
   </si>
 </sst>
 </file>
@@ -570,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,6 +1037,244 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -855,8 +1297,25 @@
     <hyperlink ref="C16" r:id="rId16" xr:uid="{CB708ABE-2E24-4234-B0A4-2651A479F21D}"/>
     <hyperlink ref="C17" r:id="rId17" xr:uid="{33AFE8E3-FC8B-4EF1-817F-89905B6343FF}"/>
     <hyperlink ref="C18" r:id="rId18" xr:uid="{59D0B267-36EA-4572-962E-7F9A49D75671}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{431FA698-9548-4AFD-BA35-BFFA574D1EC8}"/>
+    <hyperlink ref="C20" r:id="rId20" xr:uid="{92543B91-8539-4C80-8C6C-A81EF290F680}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{86F255D0-F760-459C-8452-1D1B1EB8CDC5}"/>
+    <hyperlink ref="C22" r:id="rId22" xr:uid="{B150314C-AA6C-46ED-854B-4DDF9E1E86BF}"/>
+    <hyperlink ref="C23" r:id="rId23" xr:uid="{93B541C5-3C41-49A6-A072-314B25F40A55}"/>
+    <hyperlink ref="C24" r:id="rId24" xr:uid="{C374C8A2-580B-42E0-B653-B8F0FF5550ED}"/>
+    <hyperlink ref="C25" r:id="rId25" xr:uid="{833F78B3-8231-466D-8BC6-C4C251235B65}"/>
+    <hyperlink ref="C26" r:id="rId26" xr:uid="{A1CCFB5A-71C9-4C75-A11B-59CF073C5453}"/>
+    <hyperlink ref="C27" r:id="rId27" xr:uid="{E1C6005C-A766-46A7-85C7-95D531E49505}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{FAFD8500-999F-4D3B-A58A-F2F1577A50AE}"/>
+    <hyperlink ref="C28" r:id="rId29" xr:uid="{7EBE2A80-7092-41E7-B4FF-61FDCB68A5FF}"/>
+    <hyperlink ref="C30" r:id="rId30" xr:uid="{F79E5F1F-33E1-4D62-8E17-F1FDD63F43C3}"/>
+    <hyperlink ref="C31" r:id="rId31" xr:uid="{CEE71183-8DFC-47ED-88FA-A00186F99F15}"/>
+    <hyperlink ref="C32" r:id="rId32" xr:uid="{4B004895-5E61-48B7-8E8D-224A77DD19CA}"/>
+    <hyperlink ref="C33" r:id="rId33" xr:uid="{F98998D1-2A3D-4BF9-BD5C-661A0A881EBF}"/>
+    <hyperlink ref="C34" r:id="rId34" xr:uid="{F0D4BB08-1D95-42A5-B2B0-1C3875CE003F}"/>
+    <hyperlink ref="C35" r:id="rId35" xr:uid="{4F374651-5330-4C60-AC93-B51468E32088}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>